<commit_message>
BFI, MI, 241111 modified 7
</commit_message>
<xml_diff>
--- a/R/data/quiz241111.xlsx
+++ b/R/data/quiz241111.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/Documents/class202402/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4340C16-3150-5D4F-A6C2-8AB829E11992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB868A0E-1F3F-F345-93F8-EA1C418EC464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51180" yWindow="1540" windowWidth="50880" windowHeight="26540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45120" yWindow="1360" windowWidth="50880" windowHeight="26540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="설문지 응답 시트1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2937" uniqueCount="640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3091" uniqueCount="666">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -1940,6 +1940,84 @@
   </si>
   <si>
     <t>김기원</t>
+  </si>
+  <si>
+    <t>skaskgus@gmail.com</t>
+  </si>
+  <si>
+    <t>남나현</t>
+  </si>
+  <si>
+    <t>ejsl5231@gmail.com</t>
+  </si>
+  <si>
+    <t>이유찬</t>
+  </si>
+  <si>
+    <t>a22234781@gmail.com</t>
+  </si>
+  <si>
+    <t>dlaehdghks123@gmail.com</t>
+  </si>
+  <si>
+    <t>임동환</t>
+  </si>
+  <si>
+    <t>sangim041113@gmail.com</t>
+  </si>
+  <si>
+    <t>용상임</t>
+  </si>
+  <si>
+    <t>ansk999@gmail.com</t>
+  </si>
+  <si>
+    <t>위수현</t>
+  </si>
+  <si>
+    <t>dydwndus1115@naver.com</t>
+  </si>
+  <si>
+    <t>용주연</t>
+  </si>
+  <si>
+    <t>ddoyeong0509@gmail.com</t>
+  </si>
+  <si>
+    <t>윤소영</t>
+  </si>
+  <si>
+    <t>hyeonjin0976@gmail.com</t>
+  </si>
+  <si>
+    <t>류현진</t>
+  </si>
+  <si>
+    <t>minchan6020@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">김민찬 </t>
+  </si>
+  <si>
+    <t>sshee718@gmail.com</t>
+  </si>
+  <si>
+    <t>권도운</t>
+  </si>
+  <si>
+    <t>scott1234698@naver.com</t>
+  </si>
+  <si>
+    <t>우성진</t>
+  </si>
+  <si>
+    <t>smianas20@naver.com</t>
+  </si>
+  <si>
+    <t>hhr0408@gmail.com</t>
+  </si>
+  <si>
+    <t>한혜령</t>
   </si>
 </sst>
 </file>
@@ -2360,7 +2438,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:N266">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:N280">
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="타임스탬프"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="이메일 주소"/>
@@ -2582,11 +2660,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O266"/>
+  <dimension ref="A1:O280"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D270" sqref="D270"/>
+      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E291" sqref="E291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -13546,7 +13624,581 @@
       <c r="M266" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="N266" s="23"/>
+    </row>
+    <row r="267" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A267" s="7">
+        <v>45613.43792960648</v>
+      </c>
+      <c r="B267" s="8" t="s">
+        <v>640</v>
+      </c>
+      <c r="C267" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D267" s="8">
+        <v>20202324</v>
+      </c>
+      <c r="E267" s="8" t="s">
+        <v>641</v>
+      </c>
+      <c r="F267" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G267" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H267" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="I267" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J267" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K267" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L267" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M267" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="268" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A268" s="4">
+        <v>45613.487628750001</v>
+      </c>
+      <c r="B268" s="5" t="s">
+        <v>642</v>
+      </c>
+      <c r="C268" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="D268" s="5">
+        <v>20225223</v>
+      </c>
+      <c r="E268" s="5" t="s">
+        <v>643</v>
+      </c>
+      <c r="F268" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G268" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H268" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I268" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J268" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K268" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L268" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N268" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="269" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A269" s="7">
+        <v>45613.522831111113</v>
+      </c>
+      <c r="B269" s="8" t="s">
+        <v>644</v>
+      </c>
+      <c r="C269" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D269" s="8">
+        <v>20201076</v>
+      </c>
+      <c r="E269" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="F269" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G269" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H269" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="I269" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J269" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="K269" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L269" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N269" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="270" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A270" s="4">
+        <v>45613.523186435181</v>
+      </c>
+      <c r="B270" s="5" t="s">
+        <v>645</v>
+      </c>
+      <c r="C270" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D270" s="5">
+        <v>20213533</v>
+      </c>
+      <c r="E270" s="5" t="s">
+        <v>646</v>
+      </c>
+      <c r="F270" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G270" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H270" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="I270" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J270" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K270" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="L270" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N270" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="271" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A271" s="7">
+        <v>45613.566498182874</v>
+      </c>
+      <c r="B271" s="8" t="s">
+        <v>647</v>
+      </c>
+      <c r="C271" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D271" s="8">
+        <v>20235209</v>
+      </c>
+      <c r="E271" s="8" t="s">
+        <v>648</v>
+      </c>
+      <c r="F271" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G271" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H271" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I271" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J271" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K271" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L271" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N271" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="272" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A272" s="4">
+        <v>45613.588818368051</v>
+      </c>
+      <c r="B272" s="5" t="s">
+        <v>649</v>
+      </c>
+      <c r="C272" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D272" s="5">
+        <v>20202736</v>
+      </c>
+      <c r="E272" s="5" t="s">
+        <v>650</v>
+      </c>
+      <c r="F272" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G272" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H272" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I272" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J272" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K272" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L272" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N272" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="273" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A273" s="7">
+        <v>45613.59455760417</v>
+      </c>
+      <c r="B273" s="8" t="s">
+        <v>651</v>
+      </c>
+      <c r="C273" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="D273" s="8">
+        <v>20243723</v>
+      </c>
+      <c r="E273" s="8" t="s">
+        <v>652</v>
+      </c>
+      <c r="F273" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G273" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H273" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I273" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J273" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="K273" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="L273" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N273" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="274" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A274" s="4">
+        <v>45613.635252511573</v>
+      </c>
+      <c r="B274" s="5" t="s">
+        <v>653</v>
+      </c>
+      <c r="C274" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D274" s="5">
+        <v>20242424</v>
+      </c>
+      <c r="E274" s="5" t="s">
+        <v>654</v>
+      </c>
+      <c r="F274" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G274" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H274" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I274" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J274" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K274" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L274" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M274" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="275" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A275" s="7">
+        <v>45613.643073067127</v>
+      </c>
+      <c r="B275" s="8" t="s">
+        <v>655</v>
+      </c>
+      <c r="C275" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D275" s="8">
+        <v>20192717</v>
+      </c>
+      <c r="E275" s="8" t="s">
+        <v>656</v>
+      </c>
+      <c r="F275" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G275" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H275" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="I275" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J275" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K275" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L275" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N275" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="276" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A276" s="4">
+        <v>45613.65589736111</v>
+      </c>
+      <c r="B276" s="5" t="s">
+        <v>657</v>
+      </c>
+      <c r="C276" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D276" s="5">
+        <v>20242508</v>
+      </c>
+      <c r="E276" s="5" t="s">
+        <v>658</v>
+      </c>
+      <c r="F276" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G276" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H276" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I276" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J276" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K276" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L276" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N276" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="277" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A277" s="7">
+        <v>45613.666295324074</v>
+      </c>
+      <c r="B277" s="8" t="s">
+        <v>659</v>
+      </c>
+      <c r="C277" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="D277" s="8">
+        <v>20243702</v>
+      </c>
+      <c r="E277" s="8" t="s">
+        <v>660</v>
+      </c>
+      <c r="F277" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G277" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H277" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I277" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J277" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K277" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="L277" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N277" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="278" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A278" s="4">
+        <v>45613.670301921295</v>
+      </c>
+      <c r="B278" s="5" t="s">
+        <v>661</v>
+      </c>
+      <c r="C278" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D278" s="5">
+        <v>20246633</v>
+      </c>
+      <c r="E278" s="5" t="s">
+        <v>662</v>
+      </c>
+      <c r="F278" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G278" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H278" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I278" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J278" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K278" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="L278" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M278" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="279" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A279" s="7">
+        <v>45613.699707858796</v>
+      </c>
+      <c r="B279" s="8" t="s">
+        <v>663</v>
+      </c>
+      <c r="C279" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D279" s="8">
+        <v>20233031</v>
+      </c>
+      <c r="E279" s="8" t="s">
+        <v>477</v>
+      </c>
+      <c r="F279" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G279" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H279" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I279" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="J279" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K279" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L279" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N279" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="280" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A280" s="15">
+        <v>45613.706954247682</v>
+      </c>
+      <c r="B280" s="16" t="s">
+        <v>664</v>
+      </c>
+      <c r="C280" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="D280" s="16">
+        <v>20246648</v>
+      </c>
+      <c r="E280" s="16" t="s">
+        <v>665</v>
+      </c>
+      <c r="F280" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G280" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H280" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="I280" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="J280" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="K280" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="L280" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="M280" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="N280" s="23"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
BFI, MI, 241111 modified 9
</commit_message>
<xml_diff>
--- a/R/data/quiz241111.xlsx
+++ b/R/data/quiz241111.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/Documents/class202402/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB868A0E-1F3F-F345-93F8-EA1C418EC464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8961A2-D222-374F-A678-A83F9E757A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45120" yWindow="1360" windowWidth="50880" windowHeight="26540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3091" uniqueCount="666">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3663" uniqueCount="775">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -2018,6 +2018,333 @@
   </si>
   <si>
     <t>한혜령</t>
+  </si>
+  <si>
+    <t>jennydz@naver.com</t>
+  </si>
+  <si>
+    <t>허지수</t>
+  </si>
+  <si>
+    <t>shasha4321@naver.com</t>
+  </si>
+  <si>
+    <t>정다영</t>
+  </si>
+  <si>
+    <t>20242925@hallym.ac.kr</t>
+  </si>
+  <si>
+    <t>경영학부</t>
+  </si>
+  <si>
+    <t>김민우</t>
+  </si>
+  <si>
+    <t>ann12ann1209@gmail.com</t>
+  </si>
+  <si>
+    <t>김혜원</t>
+  </si>
+  <si>
+    <t>park_minkyu@naver.com</t>
+  </si>
+  <si>
+    <t>박민규</t>
+  </si>
+  <si>
+    <t>0223wltn@naver.com</t>
+  </si>
+  <si>
+    <t>홍지수</t>
+  </si>
+  <si>
+    <t>ehddn0504@naver.com</t>
+  </si>
+  <si>
+    <t>신동우</t>
+  </si>
+  <si>
+    <t>guj2205146@gmail.com</t>
+  </si>
+  <si>
+    <t>강의주</t>
+  </si>
+  <si>
+    <t>youlove6767@naver.com</t>
+  </si>
+  <si>
+    <t>임소이</t>
+  </si>
+  <si>
+    <t>syb00syb00@naver.com</t>
+  </si>
+  <si>
+    <t>신유비</t>
+  </si>
+  <si>
+    <t>akeb110@naver.com</t>
+  </si>
+  <si>
+    <t>김은빈</t>
+  </si>
+  <si>
+    <t>b020305@naver.com</t>
+  </si>
+  <si>
+    <t>배성진</t>
+  </si>
+  <si>
+    <t>jaekyung001203@gmail.com</t>
+  </si>
+  <si>
+    <t>데이터사이언스</t>
+  </si>
+  <si>
+    <t>안재경</t>
+  </si>
+  <si>
+    <t>yohihong@gmail.com</t>
+  </si>
+  <si>
+    <t>민홍기</t>
+  </si>
+  <si>
+    <t>andy9925@naver.com</t>
+  </si>
+  <si>
+    <t>김무극</t>
+  </si>
+  <si>
+    <t>wogh1587@naver.com</t>
+  </si>
+  <si>
+    <t>현재호</t>
+  </si>
+  <si>
+    <t>ab47cd32@gmail.com</t>
+  </si>
+  <si>
+    <t>우로겸</t>
+  </si>
+  <si>
+    <t>pdh9467472@gmail.com</t>
+  </si>
+  <si>
+    <t>법</t>
+  </si>
+  <si>
+    <t>박두환</t>
+  </si>
+  <si>
+    <t>kylebusy@naver.com</t>
+  </si>
+  <si>
+    <t>이동훈</t>
+  </si>
+  <si>
+    <t>lucy011705@naver.com</t>
+  </si>
+  <si>
+    <t>이민정</t>
+  </si>
+  <si>
+    <t>ryul1128@naver.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">식품영양학과 </t>
+  </si>
+  <si>
+    <t>김률아</t>
+  </si>
+  <si>
+    <t>wizkids0418@naver.com</t>
+  </si>
+  <si>
+    <t>박혜인</t>
+  </si>
+  <si>
+    <t>tjtkdwns0909@naver.com</t>
+  </si>
+  <si>
+    <t>서상준</t>
+  </si>
+  <si>
+    <t>syuniw26@gmail.com</t>
+  </si>
+  <si>
+    <t>이서윤</t>
+  </si>
+  <si>
+    <t>dkdud4750@naver.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">심리학과 </t>
+  </si>
+  <si>
+    <t>양아영</t>
+  </si>
+  <si>
+    <t>ekzkdi12@naver.com</t>
+  </si>
+  <si>
+    <t>박정민</t>
+  </si>
+  <si>
+    <t>ncu11069@naver.com</t>
+  </si>
+  <si>
+    <t>이규민</t>
+  </si>
+  <si>
+    <t>mi3107359@gmail.com</t>
+  </si>
+  <si>
+    <t>이미진</t>
+  </si>
+  <si>
+    <t>yssong1919@naver.com</t>
+  </si>
+  <si>
+    <t>송예상</t>
+  </si>
+  <si>
+    <t>jsk991012@naver.com</t>
+  </si>
+  <si>
+    <t>김준서</t>
+  </si>
+  <si>
+    <t>kter0506@naver.com</t>
+  </si>
+  <si>
+    <t>김태은</t>
+  </si>
+  <si>
+    <t>a01028349689@gmail.com</t>
+  </si>
+  <si>
+    <t>최다인</t>
+  </si>
+  <si>
+    <t>jin050828@gmail.com</t>
+  </si>
+  <si>
+    <t>김진영</t>
+  </si>
+  <si>
+    <t>kmhhth5@gmail.com</t>
+  </si>
+  <si>
+    <t>최진호</t>
+  </si>
+  <si>
+    <t>obokboki@naver.com</t>
+  </si>
+  <si>
+    <t>최서윤</t>
+  </si>
+  <si>
+    <t>chjames2005@naver.com</t>
+  </si>
+  <si>
+    <t>최재현</t>
+  </si>
+  <si>
+    <t>leejhzzang2005@naver.com</t>
+  </si>
+  <si>
+    <t>이주현</t>
+  </si>
+  <si>
+    <t>kangdmscks@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">융합과학수사학과 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">강은찬 </t>
+  </si>
+  <si>
+    <t>taewon16@naver.com</t>
+  </si>
+  <si>
+    <t>류태원</t>
+  </si>
+  <si>
+    <t>parkjinseo23@naver.com</t>
+  </si>
+  <si>
+    <t>minsung5342@naver.com</t>
+  </si>
+  <si>
+    <t>eseses0827@naver.com</t>
+  </si>
+  <si>
+    <t>강은서</t>
+  </si>
+  <si>
+    <t>kby5432@naver.com</t>
+  </si>
+  <si>
+    <t>윤경빈</t>
+  </si>
+  <si>
+    <t>erang051216@naver.com</t>
+  </si>
+  <si>
+    <t>박이랑</t>
+  </si>
+  <si>
+    <t>siqyy2003@gmail.com</t>
+  </si>
+  <si>
+    <t>체육</t>
+  </si>
+  <si>
+    <t>양민서</t>
+  </si>
+  <si>
+    <t>sehyeon0330@naver.com</t>
+  </si>
+  <si>
+    <t>김세현</t>
+  </si>
+  <si>
+    <t>stacy4036@naver.com</t>
+  </si>
+  <si>
+    <t>최하은</t>
+  </si>
+  <si>
+    <t>youngold057@gmail.com</t>
+  </si>
+  <si>
+    <t>윤태영</t>
+  </si>
+  <si>
+    <t>ss0001234@nave.com</t>
+  </si>
+  <si>
+    <t>김세은</t>
+  </si>
+  <si>
+    <t>jkmy2516@naver.com</t>
+  </si>
+  <si>
+    <t>장석빈</t>
+  </si>
+  <si>
+    <t>haksun0217@naver.com</t>
+  </si>
+  <si>
+    <t>김학선</t>
+  </si>
+  <si>
+    <t>ysh050116@naver.com</t>
+  </si>
+  <si>
+    <t>윤시한</t>
   </si>
 </sst>
 </file>
@@ -2438,7 +2765,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:N280">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:N332">
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="타임스탬프"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="이메일 주소"/>
@@ -2660,11 +2987,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O280"/>
+  <dimension ref="A1:O332"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E291" sqref="E291"/>
+      <pane ySplit="1" topLeftCell="A273" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C336" sqref="C336"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -14198,7 +14525,2139 @@
       <c r="M280" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="N280" s="23"/>
+    </row>
+    <row r="281" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A281" s="7">
+        <v>45613.727580277773</v>
+      </c>
+      <c r="B281" s="8" t="s">
+        <v>666</v>
+      </c>
+      <c r="C281" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D281" s="8">
+        <v>20213543</v>
+      </c>
+      <c r="E281" s="8" t="s">
+        <v>667</v>
+      </c>
+      <c r="F281" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G281" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H281" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I281" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J281" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K281" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L281" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N281" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="282" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A282" s="4">
+        <v>45613.732598194445</v>
+      </c>
+      <c r="B282" s="5" t="s">
+        <v>668</v>
+      </c>
+      <c r="C282" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="D282" s="5">
+        <v>20213035</v>
+      </c>
+      <c r="E282" s="5" t="s">
+        <v>669</v>
+      </c>
+      <c r="F282" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G282" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H282" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I282" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J282" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K282" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="L282" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N282" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="283" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A283" s="7">
+        <v>45613.736584780097</v>
+      </c>
+      <c r="B283" s="8" t="s">
+        <v>670</v>
+      </c>
+      <c r="C283" s="8" t="s">
+        <v>671</v>
+      </c>
+      <c r="D283" s="8">
+        <v>20242925</v>
+      </c>
+      <c r="E283" s="8" t="s">
+        <v>672</v>
+      </c>
+      <c r="F283" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G283" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H283" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I283" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J283" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K283" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L283" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M283" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="284" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A284" s="4">
+        <v>45613.739070925927</v>
+      </c>
+      <c r="B284" s="5" t="s">
+        <v>673</v>
+      </c>
+      <c r="C284" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="D284" s="5">
+        <v>20222933</v>
+      </c>
+      <c r="E284" s="5" t="s">
+        <v>674</v>
+      </c>
+      <c r="F284" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G284" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H284" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="I284" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J284" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K284" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="L284" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N284" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="285" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A285" s="7">
+        <v>45613.748655127318</v>
+      </c>
+      <c r="B285" s="8" t="s">
+        <v>675</v>
+      </c>
+      <c r="C285" s="8" t="s">
+        <v>602</v>
+      </c>
+      <c r="D285" s="8">
+        <v>20205167</v>
+      </c>
+      <c r="E285" s="8" t="s">
+        <v>676</v>
+      </c>
+      <c r="F285" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G285" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H285" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="I285" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="J285" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K285" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="L285" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N285" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="286" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A286" s="4">
+        <v>45613.751926666664</v>
+      </c>
+      <c r="B286" s="5" t="s">
+        <v>677</v>
+      </c>
+      <c r="C286" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D286" s="5">
+        <v>20243850</v>
+      </c>
+      <c r="E286" s="5" t="s">
+        <v>678</v>
+      </c>
+      <c r="F286" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G286" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H286" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I286" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="J286" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K286" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L286" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M286" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="287" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A287" s="7">
+        <v>45613.77076407407</v>
+      </c>
+      <c r="B287" s="8" t="s">
+        <v>679</v>
+      </c>
+      <c r="C287" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="D287" s="8">
+        <v>20245186</v>
+      </c>
+      <c r="E287" s="8" t="s">
+        <v>680</v>
+      </c>
+      <c r="F287" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G287" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H287" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="I287" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J287" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K287" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="L287" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N287" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="288" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A288" s="4">
+        <v>45613.786939861107</v>
+      </c>
+      <c r="B288" s="5" t="s">
+        <v>681</v>
+      </c>
+      <c r="C288" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D288" s="5">
+        <v>20242101</v>
+      </c>
+      <c r="E288" s="5" t="s">
+        <v>682</v>
+      </c>
+      <c r="F288" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G288" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H288" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I288" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J288" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K288" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L288" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N288" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="289" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A289" s="7">
+        <v>45613.789280821758</v>
+      </c>
+      <c r="B289" s="8" t="s">
+        <v>683</v>
+      </c>
+      <c r="C289" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D289" s="8">
+        <v>20232745</v>
+      </c>
+      <c r="E289" s="8" t="s">
+        <v>684</v>
+      </c>
+      <c r="F289" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G289" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H289" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I289" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J289" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="K289" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="L289" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N289" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="290" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A290" s="4">
+        <v>45613.789776180551</v>
+      </c>
+      <c r="B290" s="5" t="s">
+        <v>685</v>
+      </c>
+      <c r="C290" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="D290" s="5">
+        <v>20234128</v>
+      </c>
+      <c r="E290" s="5" t="s">
+        <v>686</v>
+      </c>
+      <c r="F290" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G290" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H290" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I290" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J290" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K290" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L290" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M290" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="291" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A291" s="7">
+        <v>45613.812912106485</v>
+      </c>
+      <c r="B291" s="8" t="s">
+        <v>687</v>
+      </c>
+      <c r="C291" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="D291" s="8">
+        <v>20231708</v>
+      </c>
+      <c r="E291" s="8" t="s">
+        <v>688</v>
+      </c>
+      <c r="F291" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G291" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H291" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="I291" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J291" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K291" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L291" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M291" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="292" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A292" s="4">
+        <v>45613.818836134262</v>
+      </c>
+      <c r="B292" s="5" t="s">
+        <v>689</v>
+      </c>
+      <c r="C292" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D292" s="5">
+        <v>20212418</v>
+      </c>
+      <c r="E292" s="5" t="s">
+        <v>690</v>
+      </c>
+      <c r="F292" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G292" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H292" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I292" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="J292" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K292" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L292" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M292" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="293" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A293" s="7">
+        <v>45613.822115694449</v>
+      </c>
+      <c r="B293" s="8" t="s">
+        <v>691</v>
+      </c>
+      <c r="C293" s="8" t="s">
+        <v>692</v>
+      </c>
+      <c r="D293" s="8">
+        <v>20213230</v>
+      </c>
+      <c r="E293" s="8" t="s">
+        <v>693</v>
+      </c>
+      <c r="F293" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G293" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H293" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I293" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J293" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K293" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L293" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N293" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="294" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A294" s="4">
+        <v>45613.827205972222</v>
+      </c>
+      <c r="B294" s="5" t="s">
+        <v>694</v>
+      </c>
+      <c r="C294" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="D294" s="5">
+        <v>20245161</v>
+      </c>
+      <c r="E294" s="5" t="s">
+        <v>695</v>
+      </c>
+      <c r="F294" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G294" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H294" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I294" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J294" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K294" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L294" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N294" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="295" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A295" s="7">
+        <v>45613.829508055554</v>
+      </c>
+      <c r="B295" s="8" t="s">
+        <v>696</v>
+      </c>
+      <c r="C295" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="D295" s="8">
+        <v>20234110</v>
+      </c>
+      <c r="E295" s="8" t="s">
+        <v>697</v>
+      </c>
+      <c r="F295" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G295" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H295" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="I295" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J295" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K295" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L295" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M295" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="296" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A296" s="4">
+        <v>45613.853275879628</v>
+      </c>
+      <c r="B296" s="5" t="s">
+        <v>698</v>
+      </c>
+      <c r="C296" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D296" s="5">
+        <v>20192366</v>
+      </c>
+      <c r="E296" s="5" t="s">
+        <v>699</v>
+      </c>
+      <c r="F296" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G296" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H296" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I296" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J296" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K296" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L296" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M296" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="297" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A297" s="7">
+        <v>45613.85627178241</v>
+      </c>
+      <c r="B297" s="8" t="s">
+        <v>700</v>
+      </c>
+      <c r="C297" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D297" s="8">
+        <v>20242128</v>
+      </c>
+      <c r="E297" s="8" t="s">
+        <v>701</v>
+      </c>
+      <c r="F297" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G297" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H297" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I297" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J297" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K297" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L297" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N297" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="298" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A298" s="4">
+        <v>45613.859724641203</v>
+      </c>
+      <c r="B298" s="5" t="s">
+        <v>702</v>
+      </c>
+      <c r="C298" s="5" t="s">
+        <v>703</v>
+      </c>
+      <c r="D298" s="5">
+        <v>20172719</v>
+      </c>
+      <c r="E298" s="5" t="s">
+        <v>704</v>
+      </c>
+      <c r="F298" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G298" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H298" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I298" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J298" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K298" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L298" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N298" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="299" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A299" s="7">
+        <v>45613.866186504631</v>
+      </c>
+      <c r="B299" s="8" t="s">
+        <v>705</v>
+      </c>
+      <c r="C299" s="8" t="s">
+        <v>447</v>
+      </c>
+      <c r="D299" s="8">
+        <v>20212551</v>
+      </c>
+      <c r="E299" s="8" t="s">
+        <v>706</v>
+      </c>
+      <c r="F299" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G299" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H299" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="I299" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="J299" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K299" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="L299" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N299" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="300" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A300" s="4">
+        <v>45613.875365104162</v>
+      </c>
+      <c r="B300" s="5" t="s">
+        <v>707</v>
+      </c>
+      <c r="C300" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D300" s="5">
+        <v>20242997</v>
+      </c>
+      <c r="E300" s="5" t="s">
+        <v>708</v>
+      </c>
+      <c r="F300" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G300" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H300" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I300" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J300" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K300" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L300" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N300" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="301" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A301" s="7">
+        <v>45613.879153113427</v>
+      </c>
+      <c r="B301" s="8" t="s">
+        <v>709</v>
+      </c>
+      <c r="C301" s="8" t="s">
+        <v>710</v>
+      </c>
+      <c r="D301" s="8">
+        <v>20243806</v>
+      </c>
+      <c r="E301" s="8" t="s">
+        <v>711</v>
+      </c>
+      <c r="F301" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G301" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H301" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I301" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J301" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="K301" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="L301" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M301" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="302" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A302" s="4">
+        <v>45613.881010497687</v>
+      </c>
+      <c r="B302" s="5" t="s">
+        <v>712</v>
+      </c>
+      <c r="C302" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D302" s="5">
+        <v>20242327</v>
+      </c>
+      <c r="E302" s="5" t="s">
+        <v>713</v>
+      </c>
+      <c r="F302" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G302" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H302" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I302" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J302" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K302" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L302" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M302" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="303" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A303" s="7">
+        <v>45613.883699155092</v>
+      </c>
+      <c r="B303" s="8" t="s">
+        <v>714</v>
+      </c>
+      <c r="C303" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="D303" s="8">
+        <v>20244123</v>
+      </c>
+      <c r="E303" s="8" t="s">
+        <v>715</v>
+      </c>
+      <c r="F303" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G303" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H303" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I303" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J303" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K303" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L303" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M303" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="304" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A304" s="4">
+        <v>45613.891431782409</v>
+      </c>
+      <c r="B304" s="5" t="s">
+        <v>716</v>
+      </c>
+      <c r="C304" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="D304" s="5">
+        <v>20243726</v>
+      </c>
+      <c r="E304" s="5" t="s">
+        <v>717</v>
+      </c>
+      <c r="F304" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G304" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H304" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I304" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J304" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K304" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L304" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M304" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="305" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A305" s="7">
+        <v>45613.899532569441</v>
+      </c>
+      <c r="B305" s="8" t="s">
+        <v>718</v>
+      </c>
+      <c r="C305" s="8" t="s">
+        <v>719</v>
+      </c>
+      <c r="D305" s="8">
+        <v>20222122</v>
+      </c>
+      <c r="E305" s="8" t="s">
+        <v>720</v>
+      </c>
+      <c r="F305" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G305" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H305" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="I305" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J305" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K305" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="L305" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M305" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="306" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A306" s="4">
+        <v>45613.903170347221</v>
+      </c>
+      <c r="B306" s="5" t="s">
+        <v>721</v>
+      </c>
+      <c r="C306" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="D306" s="5">
+        <v>20242960</v>
+      </c>
+      <c r="E306" s="5" t="s">
+        <v>722</v>
+      </c>
+      <c r="F306" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G306" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H306" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="I306" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J306" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K306" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="L306" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N306" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="307" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A307" s="7">
+        <v>45613.904304120369</v>
+      </c>
+      <c r="B307" s="8" t="s">
+        <v>723</v>
+      </c>
+      <c r="C307" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D307" s="8">
+        <v>20231622</v>
+      </c>
+      <c r="E307" s="8" t="s">
+        <v>724</v>
+      </c>
+      <c r="F307" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G307" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H307" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I307" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J307" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K307" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="L307" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M307" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="308" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A308" s="4">
+        <v>45613.904425057874</v>
+      </c>
+      <c r="B308" s="5" t="s">
+        <v>725</v>
+      </c>
+      <c r="C308" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D308" s="5">
+        <v>20241220</v>
+      </c>
+      <c r="E308" s="5" t="s">
+        <v>726</v>
+      </c>
+      <c r="F308" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G308" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H308" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I308" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J308" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K308" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L308" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M308" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="309" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A309" s="7">
+        <v>45613.909979780088</v>
+      </c>
+      <c r="B309" s="8" t="s">
+        <v>727</v>
+      </c>
+      <c r="C309" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D309" s="8">
+        <v>20227078</v>
+      </c>
+      <c r="E309" s="8" t="s">
+        <v>728</v>
+      </c>
+      <c r="F309" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G309" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H309" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I309" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J309" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K309" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L309" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M309" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="310" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A310" s="4">
+        <v>45613.911197916663</v>
+      </c>
+      <c r="B310" s="5" t="s">
+        <v>729</v>
+      </c>
+      <c r="C310" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="D310" s="5">
+        <v>20182519</v>
+      </c>
+      <c r="E310" s="5" t="s">
+        <v>730</v>
+      </c>
+      <c r="F310" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G310" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H310" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I310" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J310" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K310" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L310" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M310" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="311" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A311" s="7">
+        <v>45613.917066539347</v>
+      </c>
+      <c r="B311" s="8" t="s">
+        <v>731</v>
+      </c>
+      <c r="C311" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D311" s="8">
+        <v>20243813</v>
+      </c>
+      <c r="E311" s="8" t="s">
+        <v>732</v>
+      </c>
+      <c r="F311" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G311" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H311" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I311" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J311" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K311" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L311" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N311" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="312" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A312" s="4">
+        <v>45613.917268148143</v>
+      </c>
+      <c r="B312" s="5" t="s">
+        <v>733</v>
+      </c>
+      <c r="C312" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="D312" s="5">
+        <v>20242635</v>
+      </c>
+      <c r="E312" s="5" t="s">
+        <v>734</v>
+      </c>
+      <c r="F312" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G312" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H312" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I312" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J312" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K312" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="L312" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N312" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="313" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A313" s="7">
+        <v>45613.924581006941</v>
+      </c>
+      <c r="B313" s="8" t="s">
+        <v>735</v>
+      </c>
+      <c r="C313" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="D313" s="8">
+        <v>20246715</v>
+      </c>
+      <c r="E313" s="8" t="s">
+        <v>736</v>
+      </c>
+      <c r="F313" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G313" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H313" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="I313" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="J313" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="K313" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="L313" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N313" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="314" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A314" s="4">
+        <v>45613.929816643518</v>
+      </c>
+      <c r="B314" s="5" t="s">
+        <v>737</v>
+      </c>
+      <c r="C314" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="D314" s="5">
+        <v>20244150</v>
+      </c>
+      <c r="E314" s="5" t="s">
+        <v>738</v>
+      </c>
+      <c r="F314" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G314" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H314" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I314" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J314" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K314" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="L314" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N314" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="315" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A315" s="7">
+        <v>45613.930131388886</v>
+      </c>
+      <c r="B315" s="8" t="s">
+        <v>739</v>
+      </c>
+      <c r="C315" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D315" s="8">
+        <v>20241236</v>
+      </c>
+      <c r="E315" s="8" t="s">
+        <v>740</v>
+      </c>
+      <c r="F315" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G315" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H315" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I315" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J315" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="K315" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="L315" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N315" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="316" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A316" s="4">
+        <v>45613.930135300921</v>
+      </c>
+      <c r="B316" s="5" t="s">
+        <v>741</v>
+      </c>
+      <c r="C316" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D316" s="5">
+        <v>20243259</v>
+      </c>
+      <c r="E316" s="5" t="s">
+        <v>742</v>
+      </c>
+      <c r="F316" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G316" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H316" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I316" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J316" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K316" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L316" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N316" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="317" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A317" s="7">
+        <v>45613.937076296294</v>
+      </c>
+      <c r="B317" s="8" t="s">
+        <v>743</v>
+      </c>
+      <c r="C317" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D317" s="8">
+        <v>20242342</v>
+      </c>
+      <c r="E317" s="8" t="s">
+        <v>744</v>
+      </c>
+      <c r="F317" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G317" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H317" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I317" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J317" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K317" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L317" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M317" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="318" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A318" s="4">
+        <v>45613.946793541661</v>
+      </c>
+      <c r="B318" s="5" t="s">
+        <v>745</v>
+      </c>
+      <c r="C318" s="5" t="s">
+        <v>746</v>
+      </c>
+      <c r="D318" s="5">
+        <v>20246904</v>
+      </c>
+      <c r="E318" s="5" t="s">
+        <v>747</v>
+      </c>
+      <c r="F318" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G318" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H318" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="I318" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J318" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K318" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L318" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M318" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="319" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A319" s="7">
+        <v>45613.947733634261</v>
+      </c>
+      <c r="B319" s="8" t="s">
+        <v>748</v>
+      </c>
+      <c r="C319" s="8" t="s">
+        <v>605</v>
+      </c>
+      <c r="D319" s="8">
+        <v>20195158</v>
+      </c>
+      <c r="E319" s="8" t="s">
+        <v>749</v>
+      </c>
+      <c r="F319" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G319" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H319" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I319" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J319" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K319" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="L319" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M319" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="320" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A320" s="4">
+        <v>45613.94797804398</v>
+      </c>
+      <c r="B320" s="5" t="s">
+        <v>750</v>
+      </c>
+      <c r="C320" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D320" s="5">
+        <v>20242824</v>
+      </c>
+      <c r="E320" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="F320" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G320" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H320" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I320" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J320" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K320" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L320" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M320" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="321" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A321" s="7">
+        <v>45613.951094398144</v>
+      </c>
+      <c r="B321" s="8" t="s">
+        <v>751</v>
+      </c>
+      <c r="C321" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D321" s="8">
+        <v>20232311</v>
+      </c>
+      <c r="E321" s="8" t="s">
+        <v>473</v>
+      </c>
+      <c r="F321" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G321" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H321" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I321" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J321" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K321" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L321" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M321" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="322" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A322" s="4">
+        <v>45613.957109768518</v>
+      </c>
+      <c r="B322" s="5" t="s">
+        <v>752</v>
+      </c>
+      <c r="C322" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D322" s="5">
+        <v>20241503</v>
+      </c>
+      <c r="E322" s="5" t="s">
+        <v>753</v>
+      </c>
+      <c r="F322" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G322" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H322" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="I322" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J322" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K322" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L322" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M322" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="323" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A323" s="7">
+        <v>45613.967410717596</v>
+      </c>
+      <c r="B323" s="8" t="s">
+        <v>754</v>
+      </c>
+      <c r="C323" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D323" s="8">
+        <v>20192737</v>
+      </c>
+      <c r="E323" s="8" t="s">
+        <v>755</v>
+      </c>
+      <c r="F323" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G323" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H323" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I323" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J323" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K323" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L323" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M323" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="324" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A324" s="4">
+        <v>45613.978996203703</v>
+      </c>
+      <c r="B324" s="5" t="s">
+        <v>756</v>
+      </c>
+      <c r="C324" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D324" s="5">
+        <v>20243223</v>
+      </c>
+      <c r="E324" s="5" t="s">
+        <v>757</v>
+      </c>
+      <c r="F324" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G324" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H324" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I324" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J324" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K324" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L324" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N324" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="325" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A325" s="7">
+        <v>45613.982120740737</v>
+      </c>
+      <c r="B325" s="8" t="s">
+        <v>758</v>
+      </c>
+      <c r="C325" s="8" t="s">
+        <v>759</v>
+      </c>
+      <c r="D325" s="8">
+        <v>20224123</v>
+      </c>
+      <c r="E325" s="8" t="s">
+        <v>760</v>
+      </c>
+      <c r="F325" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G325" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H325" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="I325" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J325" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K325" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L325" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N325" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="326" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A326" s="4">
+        <v>45613.98477466435</v>
+      </c>
+      <c r="B326" s="5" t="s">
+        <v>761</v>
+      </c>
+      <c r="C326" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="D326" s="5">
+        <v>20212609</v>
+      </c>
+      <c r="E326" s="5" t="s">
+        <v>762</v>
+      </c>
+      <c r="F326" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G326" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H326" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I326" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J326" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K326" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="L326" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M326" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="327" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A327" s="7">
+        <v>45613.990983622687</v>
+      </c>
+      <c r="B327" s="8" t="s">
+        <v>763</v>
+      </c>
+      <c r="C327" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D327" s="8">
+        <v>20227034</v>
+      </c>
+      <c r="E327" s="8" t="s">
+        <v>764</v>
+      </c>
+      <c r="F327" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G327" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H327" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I327" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J327" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="K327" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="L327" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N327" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="328" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A328" s="4">
+        <v>45613.999646331024</v>
+      </c>
+      <c r="B328" s="5" t="s">
+        <v>765</v>
+      </c>
+      <c r="C328" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D328" s="5">
+        <v>20242336</v>
+      </c>
+      <c r="E328" s="5" t="s">
+        <v>766</v>
+      </c>
+      <c r="F328" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G328" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H328" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="I328" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J328" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K328" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L328" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M328" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="329" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A329" s="7">
+        <v>45614.002101111109</v>
+      </c>
+      <c r="B329" s="8" t="s">
+        <v>767</v>
+      </c>
+      <c r="C329" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D329" s="8">
+        <v>20203211</v>
+      </c>
+      <c r="E329" s="8" t="s">
+        <v>768</v>
+      </c>
+      <c r="F329" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G329" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H329" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I329" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J329" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K329" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L329" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M329" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="330" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A330" s="4">
+        <v>45614.006403402775</v>
+      </c>
+      <c r="B330" s="5" t="s">
+        <v>769</v>
+      </c>
+      <c r="C330" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="D330" s="5">
+        <v>20191084</v>
+      </c>
+      <c r="E330" s="5" t="s">
+        <v>770</v>
+      </c>
+      <c r="F330" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G330" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H330" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I330" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J330" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K330" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="L330" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M330" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="331" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A331" s="7">
+        <v>45614.028893078706</v>
+      </c>
+      <c r="B331" s="8" t="s">
+        <v>771</v>
+      </c>
+      <c r="C331" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D331" s="8">
+        <v>20243814</v>
+      </c>
+      <c r="E331" s="8" t="s">
+        <v>772</v>
+      </c>
+      <c r="F331" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G331" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H331" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="I331" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J331" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K331" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="L331" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M331" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="332" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A332" s="15">
+        <v>45614.03261545139</v>
+      </c>
+      <c r="B332" s="16" t="s">
+        <v>773</v>
+      </c>
+      <c r="C332" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="D332" s="16">
+        <v>20246752</v>
+      </c>
+      <c r="E332" s="16" t="s">
+        <v>774</v>
+      </c>
+      <c r="F332" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="G332" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H332" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I332" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J332" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="K332" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="L332" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="M332" s="23"/>
+      <c r="N332" s="18" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>